<commit_message>
Cambios finales para QA ahora si
Cambios fianles
</commit_message>
<xml_diff>
--- a/Empeño.WindowsForms/Empeños/Reportes/ReporteEmpeños.xlsx
+++ b/Empeño.WindowsForms/Empeños/Reportes/ReporteEmpeños.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,62 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>REPORTE DE EMPEÑOS</t>
+  </si>
+  <si>
+    <t>EmpeñoId</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Es Oro</t>
+  </si>
+  <si>
+    <t>Identificacion</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>Interes</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Empleado</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Collar de Oro</t>
+  </si>
+  <si>
+    <t>Donovan Jarquin</t>
+  </si>
+  <si>
+    <t>Donovan</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +81,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,17 +111,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -68,8 +158,28 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A10:K32" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="A10:K32"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="EmpeñoId"/>
+    <tableColumn id="16" name="Fecha"/>
+    <tableColumn id="2" name="Descripcion"/>
+    <tableColumn id="3" name="Es Oro"/>
+    <tableColumn id="8" name="Identificacion"/>
+    <tableColumn id="9" name="Cliente"/>
+    <tableColumn id="10" name="Monto"/>
+    <tableColumn id="11" name="Interes"/>
+    <tableColumn id="12" name="Pendiente"/>
+    <tableColumn id="13" name="Empleado"/>
+    <tableColumn id="14" name="Estado"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +224,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +259,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +441,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="6" width="11.44140625" customWidth="1"/>
+    <col min="7" max="11" width="12.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" ht="33.6" x14ac:dyDescent="0.65">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4">
+        <v>43863</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>206800335</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>5000</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>5000</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:T4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="2321" orientation="portrait" horizontalDpi="160" verticalDpi="144" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>